<commit_message>
added blank after the task. balanced randomization between runs
</commit_message>
<xml_diff>
--- a/guess_condition_randomization.xlsx
+++ b/guess_condition_randomization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\pretest_fmri\Guess_fMRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Documents\GUESS\Guess_fMRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B604ABB-8044-43DA-BC71-CCE50FD8A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14F4B15-6D88-46A5-9569-B1217FE687BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{B6B42273-C89E-401B-BEA5-DC942271AE65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6B42273-C89E-401B-BEA5-DC942271AE65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="3">
   <si>
     <t>Read</t>
   </si>
@@ -97,7 +97,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -113,9 +113,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +153,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -259,7 +259,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,419 +409,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BA7CCC-2BF3-4AC0-914E-5571BAB9284E}">
-  <dimension ref="A1:A81"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.9296875" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>